<commit_message>
Excel import is now capable of auto detecting the type of the property from the setter and load entities from lookup tables depending on code given in Excel cell
</commit_message>
<xml_diff>
--- a/trunk/util/src/test/resources/data/xlsx/importTest.xlsx
+++ b/trunk/util/src/test/resources/data/xlsx/importTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Header of Date Column</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>This is a text cell</t>
+  </si>
+  <si>
+    <t>Header for Status</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -412,9 +418,10 @@
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -424,8 +431,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -434,6 +444,9 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>